<commit_message>
Cập nhật thống kê chi tiết hơn ở sơ đồ hình tròn, bổ sung chức năng xác thực khi xóa Habit
</commit_message>
<xml_diff>
--- a/Thiet_ke_DB.xlsx
+++ b/Thiet_ke_DB.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20417"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\School\Hk1_nam_2\2.Open_Source\AAA_Thi_Cuoi_Ky\Habit_Tracker\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36860BA-EDC6-430A-A2DD-323B28BBC9C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="các bảng"/>
+    <sheet name="các bảng" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -325,9 +331,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,7 +350,7 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color rgb="FFffff00"/>
+      <color rgb="FFFFFF00"/>
       <name val="Aptos"/>
       <family val="2"/>
     </font>
@@ -370,7 +375,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFff0000"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
@@ -396,12 +401,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00b0f0"/>
+        <fgColor rgb="FF00B0F0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffff00"/>
+        <fgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -422,16 +427,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -520,10 +525,10 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
@@ -532,13 +537,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
@@ -547,13 +552,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
@@ -564,92 +569,94 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="27">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="7" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -660,10 +667,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -701,71 +708,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -793,7 +800,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -816,11 +823,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -829,13 +836,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -845,7 +852,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -854,7 +861,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -863,7 +870,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -871,10 +878,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -939,35 +946,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" style="24" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="25" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="24" width="20.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="25" width="21.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="25" width="69.57642857142856" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="25" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="18.5546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.5546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" style="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="27.75">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="27.75" customHeight="1">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
@@ -975,7 +984,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="27.75">
+    <row r="3" spans="1:6" ht="27.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -993,7 +1002,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:6" ht="18.75" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
@@ -1001,7 +1010,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="23.25">
+    <row r="5" spans="1:6" ht="23.25" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1017,7 +1026,7 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="23.25">
+    <row r="6" spans="1:6" ht="23.25" customHeight="1">
       <c r="A6" s="9"/>
       <c r="B6" s="5" t="s">
         <v>10</v>
@@ -1033,7 +1042,7 @@
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="23.25">
+    <row r="7" spans="1:6" ht="23.25" customHeight="1">
       <c r="A7" s="9"/>
       <c r="B7" s="5" t="s">
         <v>14</v>
@@ -1049,7 +1058,7 @@
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
+    <row r="8" spans="1:6" ht="20.25" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
@@ -1057,7 +1066,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="23.25">
+    <row r="9" spans="1:6" ht="23.25" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -1071,7 +1080,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="23.25">
+    <row r="10" spans="1:6" ht="23.25" customHeight="1">
       <c r="A10" s="9"/>
       <c r="B10" s="5" t="s">
         <v>20</v>
@@ -1087,7 +1096,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="23.25">
+    <row r="11" spans="1:6" ht="23.25" customHeight="1">
       <c r="A11" s="9"/>
       <c r="B11" s="5" t="s">
         <v>24</v>
@@ -1101,7 +1110,7 @@
       <c r="E11" s="11"/>
       <c r="F11" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="23.25">
+    <row r="12" spans="1:6" ht="23.25" customHeight="1">
       <c r="A12" s="9"/>
       <c r="B12" s="5" t="s">
         <v>24</v>
@@ -1117,7 +1126,7 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="23.25">
+    <row r="13" spans="1:6" ht="23.25" customHeight="1">
       <c r="A13" s="9"/>
       <c r="B13" s="5" t="s">
         <v>7</v>
@@ -1131,7 +1140,7 @@
       <c r="E13" s="11"/>
       <c r="F13" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="23.25">
+    <row r="14" spans="1:6" ht="23.25" customHeight="1">
       <c r="A14" s="9"/>
       <c r="B14" s="5" t="s">
         <v>7</v>
@@ -1147,7 +1156,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="23.25">
+    <row r="15" spans="1:6" ht="23.25" customHeight="1">
       <c r="A15" s="9"/>
       <c r="B15" s="5" t="s">
         <v>35</v>
@@ -1161,7 +1170,7 @@
       <c r="E15" s="14"/>
       <c r="F15" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="23.25">
+    <row r="16" spans="1:6" ht="23.25" customHeight="1">
       <c r="A16" s="9"/>
       <c r="B16" s="5"/>
       <c r="C16" s="17"/>
@@ -1169,7 +1178,7 @@
       <c r="E16" s="12"/>
       <c r="F16" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="23.25">
+    <row r="17" spans="1:6" ht="23.25" customHeight="1">
       <c r="A17" s="4" t="s">
         <v>38</v>
       </c>
@@ -1183,7 +1192,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="23.25">
+    <row r="18" spans="1:6" ht="23.25" customHeight="1">
       <c r="A18" s="9"/>
       <c r="B18" s="5" t="s">
         <v>7</v>
@@ -1197,7 +1206,7 @@
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="23.25">
+    <row r="19" spans="1:6" ht="23.25" customHeight="1">
       <c r="A19" s="9"/>
       <c r="B19" s="5" t="s">
         <v>41</v>
@@ -1211,7 +1220,7 @@
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="23.25">
+    <row r="20" spans="1:6" ht="23.25" customHeight="1">
       <c r="A20" s="9"/>
       <c r="B20" s="5" t="s">
         <v>44</v>
@@ -1223,7 +1232,7 @@
       <c r="E20" s="11"/>
       <c r="F20" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="23.25">
+    <row r="21" spans="1:6" ht="23.25" customHeight="1">
       <c r="A21" s="9"/>
       <c r="B21" s="5" t="s">
         <v>44</v>
@@ -1235,7 +1244,7 @@
       <c r="E21" s="11"/>
       <c r="F21" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="23.25">
+    <row r="22" spans="1:6" ht="23.25" customHeight="1">
       <c r="A22" s="9"/>
       <c r="B22" s="18" t="s">
         <v>41</v>
@@ -1251,7 +1260,7 @@
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25">
+    <row r="23" spans="1:6" ht="20.25" customHeight="1">
       <c r="A23" s="3"/>
       <c r="B23" s="2"/>
       <c r="C23" s="3"/>
@@ -1259,7 +1268,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="23.25">
+    <row r="24" spans="1:6" ht="23.25" customHeight="1">
       <c r="A24" s="4" t="s">
         <v>49</v>
       </c>
@@ -1273,7 +1282,7 @@
       <c r="E24" s="7"/>
       <c r="F24" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="23.25">
+    <row r="25" spans="1:6" ht="23.25" customHeight="1">
       <c r="A25" s="9"/>
       <c r="B25" s="5" t="s">
         <v>50</v>
@@ -1289,7 +1298,7 @@
       </c>
       <c r="F25" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:6" ht="18.75" customHeight="1">
       <c r="A26" s="9"/>
       <c r="B26" s="5" t="s">
         <v>52</v>
@@ -1303,7 +1312,7 @@
       <c r="E26" s="14"/>
       <c r="F26" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:6" ht="18.75" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
@@ -1311,7 +1320,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:6" ht="18.75" customHeight="1">
       <c r="A28" s="4" t="s">
         <v>54</v>
       </c>
@@ -1325,7 +1334,7 @@
       <c r="E28" s="7"/>
       <c r="F28" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:6" ht="18.75" customHeight="1">
       <c r="A29" s="9"/>
       <c r="B29" s="5" t="s">
         <v>7</v>
@@ -1341,7 +1350,7 @@
       </c>
       <c r="F29" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:6" ht="18.75" customHeight="1">
       <c r="A30" s="9"/>
       <c r="B30" s="5" t="s">
         <v>56</v>
@@ -1355,7 +1364,7 @@
       <c r="E30" s="11"/>
       <c r="F30" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:6" ht="18.75" customHeight="1">
       <c r="A31" s="9"/>
       <c r="B31" s="5" t="s">
         <v>58</v>
@@ -1369,7 +1378,7 @@
       <c r="E31" s="11"/>
       <c r="F31" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:6" ht="18.75" customHeight="1">
       <c r="A32" s="9"/>
       <c r="B32" s="5" t="s">
         <v>60</v>
@@ -1385,7 +1394,7 @@
       </c>
       <c r="F32" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:6" ht="18.75" customHeight="1">
       <c r="A33" s="9"/>
       <c r="B33" s="5" t="s">
         <v>64</v>
@@ -1401,7 +1410,7 @@
       </c>
       <c r="F33" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row r="34" spans="1:6" ht="18.75" customHeight="1">
       <c r="A34" s="3"/>
       <c r="B34" s="5" t="s">
         <v>68</v>
@@ -1417,7 +1426,7 @@
       </c>
       <c r="F34" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row r="35" spans="1:6" ht="18.75" customHeight="1">
       <c r="A35" s="9"/>
       <c r="B35" s="5" t="s">
         <v>72</v>
@@ -1433,7 +1442,7 @@
       </c>
       <c r="F35" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row r="36" spans="1:6" ht="18.75" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="5" t="s">
         <v>76</v>
@@ -1449,7 +1458,7 @@
       </c>
       <c r="F36" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row r="37" spans="1:6" ht="18.75" customHeight="1">
       <c r="A37" s="3"/>
       <c r="B37" s="5" t="s">
         <v>44</v>
@@ -1463,7 +1472,7 @@
       <c r="E37" s="14"/>
       <c r="F37" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row r="38" spans="1:6" ht="18.75" customHeight="1">
       <c r="A38" s="3"/>
       <c r="B38" s="2"/>
       <c r="C38" s="3"/>
@@ -1471,7 +1480,7 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:6" ht="18.75" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="2"/>
       <c r="C39" s="3"/>
@@ -1479,7 +1488,7 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:6" ht="18.75" customHeight="1">
       <c r="A40" s="4" t="s">
         <v>82</v>
       </c>
@@ -1493,7 +1502,7 @@
       <c r="E40" s="7"/>
       <c r="F40" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row r="41" spans="1:6" ht="18.75" customHeight="1">
       <c r="A41" s="9"/>
       <c r="B41" s="5" t="s">
         <v>7</v>
@@ -1507,7 +1516,7 @@
       </c>
       <c r="F41" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:6" ht="18.75" customHeight="1">
       <c r="A42" s="9"/>
       <c r="B42" s="5" t="s">
         <v>7</v>
@@ -1521,7 +1530,7 @@
       <c r="E42" s="11"/>
       <c r="F42" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row r="43" spans="1:6" ht="18.75" customHeight="1">
       <c r="A43" s="9"/>
       <c r="B43" s="5" t="s">
         <v>87</v>
@@ -1535,7 +1544,7 @@
       <c r="E43" s="11"/>
       <c r="F43" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row r="44" spans="1:6" ht="18.75" customHeight="1">
       <c r="A44" s="3"/>
       <c r="B44" s="5" t="s">
         <v>44</v>
@@ -1551,7 +1560,7 @@
       </c>
       <c r="F44" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row r="45" spans="1:6" ht="18.75" customHeight="1">
       <c r="A45" s="3"/>
       <c r="B45" s="5" t="s">
         <v>91</v>
@@ -1567,7 +1576,7 @@
       </c>
       <c r="F45" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row r="46" spans="1:6" ht="18.75" customHeight="1">
       <c r="A46" s="3"/>
       <c r="B46" s="2"/>
       <c r="C46" s="3"/>
@@ -1575,7 +1584,7 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row r="47" spans="1:6" ht="18.75" customHeight="1">
       <c r="A47" s="3"/>
       <c r="B47" s="2"/>
       <c r="C47" s="3"/>
@@ -1583,7 +1592,7 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row r="48" spans="1:6" ht="18.75" customHeight="1">
       <c r="A48" s="4" t="s">
         <v>95</v>
       </c>
@@ -1597,7 +1606,7 @@
       <c r="E48" s="7"/>
       <c r="F48" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row r="49" spans="1:6" ht="18.75" customHeight="1">
       <c r="A49" s="23"/>
       <c r="B49" s="5" t="s">
         <v>96</v>
@@ -1611,7 +1620,7 @@
       <c r="E49" s="11"/>
       <c r="F49" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row r="50" spans="1:6" ht="18.75" customHeight="1">
       <c r="A50" s="23"/>
       <c r="B50" s="5" t="s">
         <v>99</v>

</xml_diff>